<commit_message>
added mongodb to docker compose
</commit_message>
<xml_diff>
--- a/lib/devdata/dev_tenant.xlsx
+++ b/lib/devdata/dev_tenant.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-740" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="4" r:id="rId1"/>
@@ -8095,9 +8095,9 @@
   </sheetPr>
   <dimension ref="A1:AR995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="247" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="247" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Able to hide/show in client form
</commit_message>
<xml_diff>
--- a/lib/devdata/dev_tenant.xlsx
+++ b/lib/devdata/dev_tenant.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="200">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -629,12 +629,6 @@
     <t xml:space="preserve">Field Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hidden</t>
-  </si>
-  <si>
     <t xml:space="preserve">Required</t>
   </si>
   <si>
@@ -668,7 +662,103 @@
     <t xml:space="preserve">telephone_number</t>
   </si>
   <si>
-    <t xml:space="preserve">current_address</t>
+    <t xml:space="preserve">province_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">family_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">case_history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">district_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commune_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">village_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">house</t>
+  </si>
+  <si>
+    <t xml:space="preserve">significant_family_member_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female_children_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male_children_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female_adult_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male_adult_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contract_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household_income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dependable_income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caregiver_information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">family_members_attributes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all_fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact_person_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact_person_email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact_person_mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organization_type_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">background</t>
   </si>
 </sst>
 </file>
@@ -964,7 +1054,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1189,6 +1279,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1267,7 +1361,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G1003"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1275,10 +1369,10 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="21.17"/>
   </cols>
   <sheetData>
@@ -2723,7 +2817,7 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
@@ -8053,7 +8147,7 @@
       <selection pane="bottomLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="1" style="0" width="28.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.33"/>
@@ -22280,18 +22374,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B45" activeCellId="0" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22304,122 +22396,490 @@
       <c r="C1" s="54" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="54" t="s">
-        <v>157</v>
-      </c>
-      <c r="E1" s="54" t="s">
-        <v>158</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="55" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+        <v>158</v>
+      </c>
+      <c r="C2" s="55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="55" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
+        <v>158</v>
+      </c>
+      <c r="C3" s="55" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="55" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+        <v>158</v>
+      </c>
+      <c r="C4" s="55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="55" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
+        <v>158</v>
+      </c>
+      <c r="C5" s="55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="55" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+        <v>158</v>
+      </c>
+      <c r="C6" s="55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="55" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
+        <v>158</v>
+      </c>
+      <c r="C7" s="55" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="55" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
+        <v>158</v>
+      </c>
+      <c r="C8" s="55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="55" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B9" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
+        <v>158</v>
+      </c>
+      <c r="C9" s="55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="55" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B10" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
+        <v>158</v>
+      </c>
+      <c r="C10" s="55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
+      <c r="C12" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="55" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="55" t="s">
+        <v>174</v>
+      </c>
+      <c r="B18" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="55" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="55" t="s">
+        <v>176</v>
+      </c>
+      <c r="B20" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C20" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="55" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="55" t="s">
+        <v>179</v>
+      </c>
+      <c r="B23" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="55" t="s">
+        <v>180</v>
+      </c>
+      <c r="B24" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C24" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="55" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C25" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="55" t="s">
+        <v>182</v>
+      </c>
+      <c r="B26" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C26" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="B27" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="55" t="s">
+        <v>184</v>
+      </c>
+      <c r="B28" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C28" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="55" t="s">
+        <v>185</v>
+      </c>
+      <c r="B29" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C29" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="B30" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C30" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="55" t="s">
+        <v>187</v>
+      </c>
+      <c r="B31" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="55" t="s">
+        <v>188</v>
+      </c>
+      <c r="B32" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="B33" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="B34" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C34" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C35" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="55" t="s">
+        <v>192</v>
+      </c>
+      <c r="B36" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C36" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="B37" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C37" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="B38" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C38" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C39" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="55" t="s">
+        <v>195</v>
+      </c>
+      <c r="B40" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C40" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="55" t="s">
+        <v>196</v>
+      </c>
+      <c r="B41" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C41" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="55" t="s">
+        <v>197</v>
+      </c>
+      <c r="B42" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C42" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="55" t="s">
+        <v>198</v>
+      </c>
+      <c r="B43" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C43" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="55" t="s">
+        <v>199</v>
+      </c>
+      <c r="B44" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C44" s="56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C45" s="56" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updated import rake task
</commit_message>
<xml_diff>
--- a/lib/devdata/dev_tenant.xlsx
+++ b/lib/devdata/dev_tenant.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="174">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -645,6 +645,9 @@
   </si>
   <si>
     <t xml:space="preserve">client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field</t>
   </si>
   <si>
     <t xml:space="preserve">rename</t>
@@ -1287,7 +1290,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G1003"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1298,7 +1301,7 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="21.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="14.5"/>
   </cols>
@@ -22306,7 +22309,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22346,13 +22349,19 @@
       <c r="C2" s="56" t="s">
         <v>161</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F2" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>1</v>
@@ -22360,47 +22369,65 @@
       <c r="C3" s="0" t="s">
         <v>161</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F3" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>161</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F4" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>161</v>
       </c>
+      <c r="D5" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F5" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="56" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B6" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6" s="56" t="s">
         <v>169</v>
-      </c>
-      <c r="C6" s="56" t="s">
-        <v>168</v>
       </c>
       <c r="D6" s="56" t="s">
         <v>156</v>
@@ -22409,18 +22436,18 @@
         <v>1</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="56" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B7" s="56" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="56" t="s">
         <v>172</v>
-      </c>
-      <c r="C7" s="56" t="s">
-        <v>171</v>
       </c>
       <c r="D7" s="56" t="s">
         <v>156</v>
@@ -22429,7 +22456,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change field from hide => show
</commit_message>
<xml_diff>
--- a/lib/devdata/dev_tenant.xlsx
+++ b/lib/devdata/dev_tenant.xlsx
@@ -635,7 +635,7 @@
     <t xml:space="preserve">type</t>
   </si>
   <si>
-    <t xml:space="preserve">hidden</t>
+    <t xml:space="preserve">visible</t>
   </si>
   <si>
     <t xml:space="preserve">remark</t>
@@ -22309,7 +22309,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22353,7 +22353,7 @@
         <v>162</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>163</v>
@@ -22373,7 +22373,7 @@
         <v>162</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>163</v>
@@ -22393,7 +22393,7 @@
         <v>162</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>163</v>
@@ -22413,7 +22413,7 @@
         <v>162</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>163</v>
@@ -22433,7 +22433,7 @@
         <v>156</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>171</v>
@@ -22453,7 +22453,7 @@
         <v>156</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>171</v>

</xml_diff>

<commit_message>
do not allow user to hide required field
</commit_message>
<xml_diff>
--- a/lib/devdata/dev_tenant.xlsx
+++ b/lib/devdata/dev_tenant.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="190">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -705,6 +705,15 @@
   </si>
   <si>
     <t xml:space="preserve">Family Name (Khamer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">received_by_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referral Received By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cannot hide</t>
   </si>
   <si>
     <t xml:space="preserve">family</t>
@@ -22349,10 +22358,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22595,29 +22604,29 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="56" t="s">
-        <v>182</v>
-      </c>
-      <c r="C9" s="56" t="s">
+      <c r="B9" s="57" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="E9" s="56" t="s">
-        <v>182</v>
-      </c>
-      <c r="F9" s="56" t="s">
-        <v>158</v>
+      <c r="E9" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>166</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>184</v>
@@ -22628,7 +22637,7 @@
         <v>185</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C10" s="56" t="s">
         <v>186</v>
@@ -22649,7 +22658,36 @@
         <v>0</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="56" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>189</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="56" t="s">
+        <v>158</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revert some client fiels with Kiry suggestion
</commit_message>
<xml_diff>
--- a/lib/devdata/dev_tenant.xlsx
+++ b/lib/devdata/dev_tenant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vibolteav/office/oscar-web/lib/devdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B206B4E8-67A6-B343-80D5-0BDCB2D03A10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F444D3-82C2-CB49-86F2-96198440F84B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="227">
   <si>
     <t>First Name</t>
   </si>
@@ -905,36 +905,6 @@
     <t>Address Type - Other address</t>
   </si>
   <si>
-    <t>difficulties</t>
-  </si>
-  <si>
-    <t>Difficulities</t>
-  </si>
-  <si>
-    <t>household_members</t>
-  </si>
-  <si>
-    <t>Household members</t>
-  </si>
-  <si>
-    <t>interview_locations</t>
-  </si>
-  <si>
-    <t>Interview location</t>
-  </si>
-  <si>
-    <t>hosting_number</t>
-  </si>
-  <si>
-    <t>How many are you hosting?</t>
-  </si>
-  <si>
-    <t>bic_others</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>family</t>
   </si>
   <si>
@@ -1439,7 +1409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1550,12 +1520,6 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -30496,10 +30460,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:IV35"/>
+  <dimension ref="A1:IV30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -30750,10 +30714,10 @@
         <v>164</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="E9" s="65" t="s">
         <v>164</v>
@@ -31322,12 +31286,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="72" t="s">
         <v>221</v>
       </c>
       <c r="B29" s="72" t="s">
-        <v>164</v>
+        <v>221</v>
       </c>
       <c r="C29" s="72" t="s">
         <v>222</v>
@@ -31335,194 +31299,49 @@
       <c r="D29" s="72" t="s">
         <v>222</v>
       </c>
-      <c r="E29" s="73" t="s">
-        <v>164</v>
-      </c>
-      <c r="F29" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="G29" s="74">
+      <c r="E29" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F29" s="72" t="s">
+        <v>158</v>
+      </c>
+      <c r="G29" s="73">
         <v>0</v>
       </c>
       <c r="H29" s="74">
-        <v>1</v>
-      </c>
-      <c r="I29" s="75" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="76" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="72" t="s">
+        <v>224</v>
+      </c>
+      <c r="B30" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="C30" s="72" t="s">
+        <v>225</v>
+      </c>
+      <c r="D30" s="72" t="s">
+        <v>225</v>
+      </c>
+      <c r="E30" s="72" t="s">
+        <v>224</v>
+      </c>
+      <c r="F30" s="72" t="s">
+        <v>158</v>
+      </c>
+      <c r="G30" s="73">
+        <v>0</v>
+      </c>
+      <c r="H30" s="74">
+        <v>0</v>
+      </c>
+      <c r="I30" s="75" t="s">
         <v>223</v>
-      </c>
-      <c r="B30" s="72" t="s">
-        <v>164</v>
-      </c>
-      <c r="C30" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="D30" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="E30" s="73" t="s">
-        <v>164</v>
-      </c>
-      <c r="F30" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="G30" s="74">
-        <v>0</v>
-      </c>
-      <c r="H30" s="74">
-        <v>1</v>
-      </c>
-      <c r="I30" s="75" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="72" t="s">
-        <v>225</v>
-      </c>
-      <c r="B31" s="72" t="s">
-        <v>164</v>
-      </c>
-      <c r="C31" s="72" t="s">
-        <v>226</v>
-      </c>
-      <c r="D31" s="72" t="s">
-        <v>226</v>
-      </c>
-      <c r="E31" s="73" t="s">
-        <v>164</v>
-      </c>
-      <c r="F31" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="G31" s="74">
-        <v>0</v>
-      </c>
-      <c r="H31" s="74">
-        <v>1</v>
-      </c>
-      <c r="I31" s="75" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="72" t="s">
-        <v>227</v>
-      </c>
-      <c r="B32" s="72" t="s">
-        <v>164</v>
-      </c>
-      <c r="C32" s="72" t="s">
-        <v>228</v>
-      </c>
-      <c r="D32" s="72" t="s">
-        <v>228</v>
-      </c>
-      <c r="E32" s="73" t="s">
-        <v>164</v>
-      </c>
-      <c r="F32" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="G32" s="74">
-        <v>0</v>
-      </c>
-      <c r="H32" s="74">
-        <v>1</v>
-      </c>
-      <c r="I32" s="75" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="72" t="s">
-        <v>229</v>
-      </c>
-      <c r="B33" s="72" t="s">
-        <v>164</v>
-      </c>
-      <c r="C33" s="72" t="s">
-        <v>230</v>
-      </c>
-      <c r="D33" s="72" t="s">
-        <v>230</v>
-      </c>
-      <c r="E33" s="73" t="s">
-        <v>164</v>
-      </c>
-      <c r="F33" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="G33" s="74">
-        <v>0</v>
-      </c>
-      <c r="H33" s="74">
-        <v>1</v>
-      </c>
-      <c r="I33" s="75" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="76" t="s">
-        <v>231</v>
-      </c>
-      <c r="B34" s="76" t="s">
-        <v>231</v>
-      </c>
-      <c r="C34" s="76" t="s">
-        <v>232</v>
-      </c>
-      <c r="D34" s="76" t="s">
-        <v>232</v>
-      </c>
-      <c r="E34" s="76" t="s">
-        <v>231</v>
-      </c>
-      <c r="F34" s="76" t="s">
-        <v>158</v>
-      </c>
-      <c r="G34" s="77">
-        <v>0</v>
-      </c>
-      <c r="H34" s="78">
-        <v>0</v>
-      </c>
-      <c r="I34" s="80" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="76" t="s">
-        <v>234</v>
-      </c>
-      <c r="B35" s="76" t="s">
-        <v>231</v>
-      </c>
-      <c r="C35" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="D35" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="E35" s="76" t="s">
-        <v>234</v>
-      </c>
-      <c r="F35" s="76" t="s">
-        <v>158</v>
-      </c>
-      <c r="G35" s="77">
-        <v>0</v>
-      </c>
-      <c r="H35" s="78">
-        <v>0</v>
-      </c>
-      <c r="I35" s="79" t="s">
-        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated dev seed data
</commit_message>
<xml_diff>
--- a/lib/devdata/dev_tenant.xlsx
+++ b/lib/devdata/dev_tenant.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="245">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -839,6 +839,48 @@
     <t xml:space="preserve">Address Type - Other address</t>
   </si>
   <si>
+    <t xml:space="preserve">province_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Province</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">district_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commune_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">village_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Street Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">house_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">House Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">current_address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">family</t>
   </si>
   <si>
@@ -864,7 +906,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="M/\D/&quot;YYYY&quot;"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -970,6 +1012,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -985,7 +1034,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1040,13 +1089,6 @@
       <right style="thin"/>
       <top style="hair"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1127,7 +1169,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1248,7 +1290,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1256,7 +1298,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1264,7 +1310,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1272,19 +1322,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1300,16 +1342,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -1418,7 +1464,7 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="44.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="44.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="21.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="8" style="1" width="8.83"/>
@@ -29203,10 +29249,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30060,61 +30106,277 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="B30" s="46" t="s">
-        <v>226</v>
+      <c r="B30" s="41" t="s">
+        <v>164</v>
       </c>
       <c r="C30" s="46" t="s">
         <v>227</v>
       </c>
-      <c r="D30" s="46" t="s">
-        <v>227</v>
-      </c>
-      <c r="E30" s="46" t="s">
-        <v>226</v>
-      </c>
-      <c r="F30" s="46" t="s">
+      <c r="D30" s="26"/>
+      <c r="E30" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="F30" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="G30" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="26"/>
+      <c r="E31" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="F31" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="G31" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="41" t="s">
+        <v>230</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C32" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="26"/>
+      <c r="E32" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="F32" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="G32" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="26"/>
+      <c r="E33" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="F33" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="G33" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="D34" s="26"/>
+      <c r="E34" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="F34" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="G34" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="B35" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="D35" s="26"/>
+      <c r="E35" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="G35" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" s="46" t="s">
+        <v>237</v>
+      </c>
+      <c r="D36" s="26"/>
+      <c r="E36" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="F36" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="G36" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" s="46" t="s">
+        <v>239</v>
+      </c>
+      <c r="D37" s="26"/>
+      <c r="E37" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="F37" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="G37" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="C38" s="47" t="s">
+        <v>241</v>
+      </c>
+      <c r="D38" s="47" t="s">
+        <v>241</v>
+      </c>
+      <c r="E38" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="F38" s="47" t="s">
         <v>158</v>
       </c>
-      <c r="G30" s="47" t="n">
+      <c r="G38" s="48" t="n">
         <v>0</v>
       </c>
-      <c r="H30" s="48" t="n">
+      <c r="H38" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="I30" s="49" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="46" t="s">
-        <v>229</v>
-      </c>
-      <c r="B31" s="46" t="s">
-        <v>226</v>
-      </c>
-      <c r="C31" s="46" t="s">
-        <v>230</v>
-      </c>
-      <c r="D31" s="46" t="s">
-        <v>230</v>
-      </c>
-      <c r="E31" s="46" t="s">
-        <v>229</v>
-      </c>
-      <c r="F31" s="46" t="s">
+      <c r="I38" s="50" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="B39" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="C39" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="D39" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="E39" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="F39" s="47" t="s">
         <v>158</v>
       </c>
-      <c r="G31" s="47" t="n">
+      <c r="G39" s="48" t="n">
         <v>0</v>
       </c>
-      <c r="H31" s="48" t="n">
+      <c r="H39" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="I31" s="50" t="s">
-        <v>228</v>
+      <c r="I39" s="51" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hide client what3words field
</commit_message>
<xml_diff>
--- a/lib/devdata/dev_tenant.xlsx
+++ b/lib/devdata/dev_tenant.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="247">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -881,6 +881,12 @@
     <t xml:space="preserve">Address Type</t>
   </si>
   <si>
+    <t xml:space="preserve">what3words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What3Words</t>
+  </si>
+  <si>
     <t xml:space="preserve">family</t>
   </si>
   <si>
@@ -29249,10 +29255,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30322,49 +30328,47 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="41" t="s">
         <v>240</v>
       </c>
-      <c r="B38" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="C38" s="47" t="s">
+      <c r="B38" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C38" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="D38" s="47" t="s">
-        <v>241</v>
-      </c>
-      <c r="E38" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="F38" s="47" t="s">
-        <v>158</v>
-      </c>
-      <c r="G38" s="48" t="n">
+      <c r="D38" s="26"/>
+      <c r="E38" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="F38" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="G38" s="43" t="n">
         <v>0</v>
       </c>
-      <c r="H38" s="49" t="n">
+      <c r="H38" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="I38" s="50" t="s">
-        <v>242</v>
+      <c r="I38" s="44" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="47" t="s">
+        <v>242</v>
+      </c>
+      <c r="B39" s="47" t="s">
+        <v>242</v>
+      </c>
+      <c r="C39" s="47" t="s">
         <v>243</v>
       </c>
-      <c r="B39" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="C39" s="47" t="s">
-        <v>244</v>
-      </c>
       <c r="D39" s="47" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E39" s="47" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F39" s="47" t="s">
         <v>158</v>
@@ -30375,8 +30379,37 @@
       <c r="H39" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="I39" s="51" t="s">
+      <c r="I39" s="50" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="47" t="s">
+        <v>245</v>
+      </c>
+      <c r="B40" s="47" t="s">
         <v>242</v>
+      </c>
+      <c r="C40" s="47" t="s">
+        <v>246</v>
+      </c>
+      <c r="D40" s="47" t="s">
+        <v>246</v>
+      </c>
+      <c r="E40" s="47" t="s">
+        <v>245</v>
+      </c>
+      <c r="F40" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="G40" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" s="51" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hide client school information
</commit_message>
<xml_diff>
--- a/lib/devdata/dev_tenant.xlsx
+++ b/lib/devdata/dev_tenant.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="249">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -887,13 +887,19 @@
     <t xml:space="preserve">What3Words</t>
   </si>
   <si>
+    <t xml:space="preserve">client_school_information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client / School Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hide section</t>
+  </si>
+  <si>
     <t xml:space="preserve">family</t>
   </si>
   <si>
     <t xml:space="preserve">Families</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hide section</t>
   </si>
   <si>
     <t xml:space="preserve">partner</t>
@@ -29255,10 +29261,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30359,14 +30365,12 @@
         <v>242</v>
       </c>
       <c r="B39" s="47" t="s">
-        <v>242</v>
+        <v>164</v>
       </c>
       <c r="C39" s="47" t="s">
         <v>243</v>
       </c>
-      <c r="D39" s="47" t="s">
-        <v>243</v>
-      </c>
+      <c r="D39" s="47"/>
       <c r="E39" s="47" t="s">
         <v>242</v>
       </c>
@@ -30388,7 +30392,7 @@
         <v>245</v>
       </c>
       <c r="B40" s="47" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C40" s="47" t="s">
         <v>246</v>
@@ -30408,7 +30412,36 @@
       <c r="H40" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="I40" s="51" t="s">
+      <c r="I40" s="50" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="47" t="s">
+        <v>247</v>
+      </c>
+      <c r="B41" s="47" t="s">
+        <v>245</v>
+      </c>
+      <c r="C41" s="47" t="s">
+        <v>248</v>
+      </c>
+      <c r="D41" s="47" t="s">
+        <v>248</v>
+      </c>
+      <c r="E41" s="47" t="s">
+        <v>247</v>
+      </c>
+      <c r="F41" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="G41" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="51" t="s">
         <v>244</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated data for deployment
</commit_message>
<xml_diff>
--- a/lib/devdata/dev_tenant.xlsx
+++ b/lib/devdata/dev_tenant.xlsx
@@ -29263,8 +29263,8 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
hide/show referee address and grouping brc address
</commit_message>
<xml_diff>
--- a/lib/devdata/dev_tenant.xlsx
+++ b/lib/devdata/dev_tenant.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="247">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -758,37 +758,37 @@
     <t xml:space="preserve">current_island</t>
   </si>
   <si>
-    <t xml:space="preserve">Island - Current address</t>
+    <t xml:space="preserve">Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">client_current_address</t>
   </si>
   <si>
     <t xml:space="preserve">current_street</t>
   </si>
   <si>
-    <t xml:space="preserve">Street - Current address</t>
-  </si>
-  <si>
     <t xml:space="preserve">current_po_box</t>
   </si>
   <si>
-    <t xml:space="preserve">PO BOX - Current address</t>
+    <t xml:space="preserve">PO BOX</t>
   </si>
   <si>
     <t xml:space="preserve">current_city</t>
   </si>
   <si>
-    <t xml:space="preserve">City - Current address</t>
+    <t xml:space="preserve">City</t>
   </si>
   <si>
     <t xml:space="preserve">current_settlement</t>
   </si>
   <si>
-    <t xml:space="preserve">Settlement - Current address</t>
+    <t xml:space="preserve">Settlement</t>
   </si>
   <si>
     <t xml:space="preserve">current_resident_own_or_rent</t>
   </si>
   <si>
-    <t xml:space="preserve">Owned or Rented - Current address</t>
+    <t xml:space="preserve">Owned or Rented</t>
   </si>
   <si>
     <t xml:space="preserve">current_household_type</t>
@@ -800,43 +800,34 @@
     <t xml:space="preserve">island2</t>
   </si>
   <si>
-    <t xml:space="preserve">Island - Other address</t>
+    <t xml:space="preserve">client_other_address</t>
   </si>
   <si>
     <t xml:space="preserve">street2</t>
   </si>
   <si>
-    <t xml:space="preserve">Street - Other address</t>
-  </si>
-  <si>
     <t xml:space="preserve">po_box2</t>
   </si>
   <si>
-    <t xml:space="preserve">Zip - Other address</t>
+    <t xml:space="preserve">Zip</t>
   </si>
   <si>
     <t xml:space="preserve">city2</t>
   </si>
   <si>
-    <t xml:space="preserve">City - Other address</t>
-  </si>
-  <si>
     <t xml:space="preserve">settlement2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Settlement - Other address</t>
   </si>
   <si>
     <t xml:space="preserve">resident_own_or_rent2</t>
   </si>
   <si>
-    <t xml:space="preserve">Owned, Rented or Temporary - Other address</t>
+    <t xml:space="preserve">Owned, Rented or Temporary</t>
   </si>
   <si>
     <t xml:space="preserve">household_type2</t>
   </si>
   <si>
-    <t xml:space="preserve">Address Type - Other address</t>
+    <t xml:space="preserve">Address Type</t>
   </si>
   <si>
     <t xml:space="preserve">province_id</t>
@@ -878,9 +869,6 @@
     <t xml:space="preserve">address_type</t>
   </si>
   <si>
-    <t xml:space="preserve">Address Type</t>
-  </si>
-  <si>
     <t xml:space="preserve">what3words</t>
   </si>
   <si>
@@ -894,6 +882,12 @@
   </si>
   <si>
     <t xml:space="preserve">hide section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">referee_address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referee</t>
   </si>
   <si>
     <t xml:space="preserve">family</t>
@@ -29261,10 +29255,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B28" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29725,7 +29719,7 @@
         <v>199</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>167</v>
@@ -29742,19 +29736,19 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="41" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B17" s="41" t="s">
         <v>164</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>201</v>
+        <v>55</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>164</v>
+        <v>55</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>200</v>
       </c>
       <c r="F17" s="42" t="s">
         <v>167</v>
@@ -29782,8 +29776,8 @@
       <c r="D18" s="45" t="s">
         <v>203</v>
       </c>
-      <c r="E18" s="42" t="s">
-        <v>164</v>
+      <c r="E18" s="24" t="s">
+        <v>200</v>
       </c>
       <c r="F18" s="42" t="s">
         <v>167</v>
@@ -29811,8 +29805,8 @@
       <c r="D19" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="E19" s="42" t="s">
-        <v>164</v>
+      <c r="E19" s="24" t="s">
+        <v>200</v>
       </c>
       <c r="F19" s="42" t="s">
         <v>167</v>
@@ -29840,8 +29834,8 @@
       <c r="D20" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="E20" s="42" t="s">
-        <v>164</v>
+      <c r="E20" s="24" t="s">
+        <v>200</v>
       </c>
       <c r="F20" s="42" t="s">
         <v>167</v>
@@ -29869,8 +29863,8 @@
       <c r="D21" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="E21" s="42" t="s">
-        <v>164</v>
+      <c r="E21" s="24" t="s">
+        <v>200</v>
       </c>
       <c r="F21" s="42" t="s">
         <v>167</v>
@@ -29898,8 +29892,8 @@
       <c r="D22" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="E22" s="42" t="s">
-        <v>164</v>
+      <c r="E22" s="24" t="s">
+        <v>200</v>
       </c>
       <c r="F22" s="42" t="s">
         <v>167</v>
@@ -29922,13 +29916,13 @@
         <v>164</v>
       </c>
       <c r="C23" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="E23" s="24" t="s">
         <v>213</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>164</v>
       </c>
       <c r="F23" s="24" t="s">
         <v>167</v>
@@ -29951,13 +29945,13 @@
         <v>164</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>215</v>
+        <v>55</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>215</v>
-      </c>
-      <c r="E24" s="42" t="s">
-        <v>164</v>
+        <v>55</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>213</v>
       </c>
       <c r="F24" s="42" t="s">
         <v>167</v>
@@ -29974,19 +29968,19 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B25" s="41" t="s">
         <v>164</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="E25" s="42" t="s">
-        <v>164</v>
+        <v>216</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>213</v>
       </c>
       <c r="F25" s="42" t="s">
         <v>167</v>
@@ -30003,19 +29997,19 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B26" s="41" t="s">
         <v>164</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="E26" s="42" t="s">
-        <v>164</v>
+        <v>205</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>213</v>
       </c>
       <c r="F26" s="42" t="s">
         <v>167</v>
@@ -30032,19 +30026,19 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="41" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B27" s="41" t="s">
         <v>164</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="E27" s="42" t="s">
-        <v>164</v>
+        <v>207</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>213</v>
       </c>
       <c r="F27" s="42" t="s">
         <v>167</v>
@@ -30061,19 +30055,19 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="41" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>164</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="E28" s="42" t="s">
-        <v>164</v>
+        <v>220</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>213</v>
       </c>
       <c r="F28" s="42" t="s">
         <v>167</v>
@@ -30090,19 +30084,19 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="41" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B29" s="41" t="s">
         <v>164</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="E29" s="42" t="s">
-        <v>164</v>
+        <v>222</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>213</v>
       </c>
       <c r="F29" s="42" t="s">
         <v>167</v>
@@ -30119,13 +30113,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="41" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B30" s="41" t="s">
         <v>164</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D30" s="26"/>
       <c r="E30" s="42" t="s">
@@ -30141,12 +30135,12 @@
         <v>0</v>
       </c>
       <c r="I30" s="44" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="41" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B31" s="41" t="s">
         <v>164</v>
@@ -30168,12 +30162,12 @@
         <v>0</v>
       </c>
       <c r="I31" s="44" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="41" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B32" s="41" t="s">
         <v>164</v>
@@ -30195,12 +30189,12 @@
         <v>0</v>
       </c>
       <c r="I32" s="44" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="41" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B33" s="41" t="s">
         <v>164</v>
@@ -30222,18 +30216,18 @@
         <v>0</v>
       </c>
       <c r="I33" s="44" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="41" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B34" s="41" t="s">
         <v>164</v>
       </c>
       <c r="C34" s="46" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="42" t="s">
@@ -30249,18 +30243,18 @@
         <v>0</v>
       </c>
       <c r="I34" s="44" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="41" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B35" s="41" t="s">
         <v>164</v>
       </c>
       <c r="C35" s="46" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="42" t="s">
@@ -30276,18 +30270,18 @@
         <v>0</v>
       </c>
       <c r="I35" s="44" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="41" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B36" s="41" t="s">
         <v>164</v>
       </c>
       <c r="C36" s="46" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D36" s="26"/>
       <c r="E36" s="42" t="s">
@@ -30303,18 +30297,18 @@
         <v>0</v>
       </c>
       <c r="I36" s="44" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="41" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B37" s="41" t="s">
         <v>164</v>
       </c>
       <c r="C37" s="46" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="D37" s="26"/>
       <c r="E37" s="42" t="s">
@@ -30330,18 +30324,18 @@
         <v>0</v>
       </c>
       <c r="I37" s="44" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="41" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B38" s="41" t="s">
         <v>164</v>
       </c>
       <c r="C38" s="46" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D38" s="26"/>
       <c r="E38" s="42" t="s">
@@ -30357,22 +30351,22 @@
         <v>0</v>
       </c>
       <c r="I38" s="44" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="47" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B39" s="47" t="s">
         <v>164</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D39" s="47"/>
       <c r="E39" s="47" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F39" s="47" t="s">
         <v>158</v>
@@ -30384,24 +30378,22 @@
         <v>0</v>
       </c>
       <c r="I39" s="50" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="47" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B40" s="47" t="s">
-        <v>245</v>
-      </c>
-      <c r="C40" s="47" t="s">
-        <v>246</v>
-      </c>
-      <c r="D40" s="47" t="s">
-        <v>246</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="D40" s="47"/>
       <c r="E40" s="47" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F40" s="47" t="s">
         <v>158</v>
@@ -30413,24 +30405,24 @@
         <v>0</v>
       </c>
       <c r="I40" s="50" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="47" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B41" s="47" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C41" s="47" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D41" s="47" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E41" s="47" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F41" s="47" t="s">
         <v>158</v>
@@ -30441,8 +30433,37 @@
       <c r="H41" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="I41" s="51" t="s">
-        <v>244</v>
+      <c r="I41" s="50" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="47" t="s">
+        <v>245</v>
+      </c>
+      <c r="B42" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="C42" s="47" t="s">
+        <v>246</v>
+      </c>
+      <c r="D42" s="47" t="s">
+        <v>246</v>
+      </c>
+      <c r="E42" s="47" t="s">
+        <v>245</v>
+      </c>
+      <c r="F42" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="G42" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="51" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
client form: rename relevant_referral_information
</commit_message>
<xml_diff>
--- a/lib/devdata/dev_tenant.xlsx
+++ b/lib/devdata/dev_tenant.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="253">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -693,6 +693,12 @@
   </si>
   <si>
     <t xml:space="preserve">Family Name (Latin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relevant_referral_information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client's referral note</t>
   </si>
   <si>
     <t xml:space="preserve">presented_id</t>
@@ -29278,10 +29284,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29478,49 +29484,45 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="D7" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="E7" s="29" t="s">
+      <c r="D7" s="0"/>
+      <c r="E7" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="5" t="n">
+      <c r="H7" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>180</v>
-      </c>
+      <c r="I7" s="34"/>
       <c r="J7" s="29" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>165</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>165</v>
@@ -29535,29 +29537,29 @@
         <v>1</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="26" t="s">
         <v>185</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="E9" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="E9" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="29" t="s">
         <v>168</v>
       </c>
       <c r="G9" s="5" t="n">
@@ -29566,41 +29568,41 @@
       <c r="H9" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="5"/>
+      <c r="I9" s="5" t="s">
+        <v>182</v>
+      </c>
       <c r="J9" s="29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>187</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>188</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="G10" s="8" t="n">
+      <c r="G10" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H10" s="8" t="n">
+      <c r="H10" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>181</v>
+      <c r="I10" s="5"/>
+      <c r="J10" s="29" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29629,24 +29631,24 @@
         <v>1</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="37" t="s">
         <v>191</v>
       </c>
       <c r="B12" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="26" t="s">
         <v>192</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E12" s="38" t="s">
         <v>165</v>
@@ -29660,20 +29662,22 @@
       <c r="H12" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="8"/>
+      <c r="I12" s="5" t="s">
+        <v>182</v>
+      </c>
       <c r="J12" s="8" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B13" s="37" t="s">
         <v>165</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>68</v>
+        <v>194</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>195</v>
@@ -29702,10 +29706,12 @@
       <c r="B14" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="D14" s="0"/>
       <c r="E14" s="38" t="s">
         <v>165</v>
       </c>
@@ -29716,26 +29722,24 @@
         <v>0</v>
       </c>
       <c r="H14" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="39" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="37" t="s">
-        <v>199</v>
       </c>
       <c r="B15" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>200</v>
-      </c>
+      <c r="C15" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="D15" s="0"/>
       <c r="E15" s="38" t="s">
         <v>165</v>
       </c>
@@ -29746,20 +29750,18 @@
         <v>0</v>
       </c>
       <c r="H15" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>180</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I15" s="8"/>
       <c r="J15" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="37" t="s">
         <v>165</v>
       </c>
       <c r="C16" s="26" t="s">
@@ -29768,23 +29770,23 @@
       <c r="D16" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="G16" s="41" t="n">
+      <c r="G16" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="H16" s="5" t="n">
+      <c r="H16" s="8" t="n">
         <v>1</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="J16" s="29" t="s">
-        <v>181</v>
+        <v>182</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29801,7 +29803,7 @@
         <v>204</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>168</v>
@@ -29813,59 +29815,59 @@
         <v>1</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J17" s="29" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="42" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="B18" s="42" t="s">
-        <v>165</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>55</v>
-      </c>
       <c r="D18" s="26" t="s">
-        <v>55</v>
+        <v>206</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="F18" s="43" t="s">
+        <v>207</v>
+      </c>
+      <c r="F18" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="G18" s="44" t="n">
+      <c r="G18" s="41" t="n">
         <v>0</v>
       </c>
-      <c r="H18" s="45" t="n">
+      <c r="H18" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="J18" s="45" t="s">
-        <v>181</v>
+        <v>182</v>
+      </c>
+      <c r="J18" s="29" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="42" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B19" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="C19" s="46" t="s">
-        <v>208</v>
-      </c>
-      <c r="D19" s="46" t="s">
-        <v>208</v>
+      <c r="C19" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>55</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F19" s="43" t="s">
         <v>168</v>
@@ -29877,10 +29879,10 @@
         <v>1</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J19" s="45" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29890,14 +29892,14 @@
       <c r="B20" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="46" t="s">
         <v>210</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F20" s="43" t="s">
         <v>168</v>
@@ -29909,10 +29911,10 @@
         <v>1</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J20" s="45" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29929,7 +29931,7 @@
         <v>212</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F21" s="43" t="s">
         <v>168</v>
@@ -29941,10 +29943,10 @@
         <v>1</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J21" s="45" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29961,7 +29963,7 @@
         <v>214</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F22" s="43" t="s">
         <v>168</v>
@@ -29973,10 +29975,10 @@
         <v>1</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J22" s="45" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29993,7 +29995,7 @@
         <v>216</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F23" s="43" t="s">
         <v>168</v>
@@ -30005,91 +30007,91 @@
         <v>1</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J23" s="45" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="42" t="s">
         <v>165</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="F24" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="F24" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="G24" s="41" t="n">
+      <c r="G24" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="H24" s="5" t="n">
+      <c r="H24" s="45" t="n">
         <v>1</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="J24" s="29" t="s">
-        <v>181</v>
+        <v>182</v>
+      </c>
+      <c r="J24" s="45" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="24" t="s">
         <v>165</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>55</v>
+        <v>206</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>55</v>
+        <v>206</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="F25" s="43" t="s">
+        <v>220</v>
+      </c>
+      <c r="F25" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="G25" s="44" t="n">
+      <c r="G25" s="41" t="n">
         <v>0</v>
       </c>
-      <c r="H25" s="45" t="n">
+      <c r="H25" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="J25" s="45" t="s">
-        <v>181</v>
+        <v>182</v>
+      </c>
+      <c r="J25" s="29" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="42" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B26" s="42" t="s">
         <v>165</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>221</v>
+        <v>55</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>221</v>
+        <v>55</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F26" s="43" t="s">
         <v>168</v>
@@ -30101,10 +30103,10 @@
         <v>1</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J26" s="45" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30115,13 +30117,13 @@
         <v>165</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F27" s="43" t="s">
         <v>168</v>
@@ -30133,15 +30135,15 @@
         <v>1</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J27" s="45" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="42" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B28" s="42" t="s">
         <v>165</v>
@@ -30153,7 +30155,7 @@
         <v>212</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F28" s="43" t="s">
         <v>168</v>
@@ -30165,27 +30167,27 @@
         <v>1</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J28" s="45" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="42" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B29" s="42" t="s">
         <v>165</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F29" s="43" t="s">
         <v>168</v>
@@ -30197,10 +30199,10 @@
         <v>1</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J29" s="45" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30217,7 +30219,7 @@
         <v>227</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F30" s="43" t="s">
         <v>168</v>
@@ -30229,10 +30231,10 @@
         <v>1</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J30" s="45" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30242,12 +30244,14 @@
       <c r="B31" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="C31" s="47" t="s">
+      <c r="C31" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="D31" s="26"/>
-      <c r="E31" s="43" t="s">
-        <v>165</v>
+      <c r="D31" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>220</v>
       </c>
       <c r="F31" s="43" t="s">
         <v>168</v>
@@ -30256,13 +30260,13 @@
         <v>0</v>
       </c>
       <c r="H31" s="45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J31" s="45" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30273,7 +30277,7 @@
         <v>165</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>52</v>
+        <v>231</v>
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="43" t="s">
@@ -30289,21 +30293,21 @@
         <v>0</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J32" s="45" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="42" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B33" s="42" t="s">
         <v>165</v>
       </c>
       <c r="C33" s="47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="43" t="s">
@@ -30319,21 +30323,21 @@
         <v>0</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J33" s="45" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="42" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B34" s="42" t="s">
         <v>165</v>
       </c>
       <c r="C34" s="47" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="43" t="s">
@@ -30349,21 +30353,21 @@
         <v>0</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J34" s="45" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="42" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B35" s="42" t="s">
         <v>165</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>234</v>
+        <v>56</v>
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="43" t="s">
@@ -30379,10 +30383,10 @@
         <v>0</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J35" s="45" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30409,10 +30413,10 @@
         <v>0</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J36" s="45" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30439,10 +30443,10 @@
         <v>0</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J37" s="45" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30453,7 +30457,7 @@
         <v>165</v>
       </c>
       <c r="C38" s="47" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="D38" s="26"/>
       <c r="E38" s="43" t="s">
@@ -30469,21 +30473,21 @@
         <v>0</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J38" s="45" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="42" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B39" s="42" t="s">
         <v>165</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="D39" s="26"/>
       <c r="E39" s="43" t="s">
@@ -30499,55 +30503,55 @@
         <v>0</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J39" s="45" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="48" t="s">
+      <c r="A40" s="42" t="s">
         <v>242</v>
       </c>
-      <c r="B40" s="48" t="s">
+      <c r="B40" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="C40" s="48" t="s">
+      <c r="C40" s="47" t="s">
         <v>243</v>
       </c>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48" t="s">
-        <v>242</v>
-      </c>
-      <c r="F40" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="G40" s="49" t="n">
+      <c r="D40" s="26"/>
+      <c r="E40" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="F40" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="G40" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="H40" s="50" t="n">
+      <c r="H40" s="45" t="n">
         <v>0</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="J40" s="51" t="s">
-        <v>244</v>
+        <v>182</v>
+      </c>
+      <c r="J40" s="45" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="48" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B41" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="C41" s="22" t="s">
-        <v>246</v>
+      <c r="C41" s="48" t="s">
+        <v>245</v>
       </c>
       <c r="D41" s="48"/>
       <c r="E41" s="48" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>158</v>
@@ -30559,10 +30563,10 @@
         <v>0</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J41" s="51" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30570,14 +30574,12 @@
         <v>247</v>
       </c>
       <c r="B42" s="48" t="s">
-        <v>247</v>
-      </c>
-      <c r="C42" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="D42" s="48" t="s">
-        <v>248</v>
-      </c>
+      <c r="D42" s="48"/>
       <c r="E42" s="48" t="s">
         <v>247</v>
       </c>
@@ -30591,10 +30593,10 @@
         <v>0</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J42" s="51" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30602,7 +30604,7 @@
         <v>249</v>
       </c>
       <c r="B43" s="48" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C43" s="48" t="s">
         <v>250</v>
@@ -30623,10 +30625,42 @@
         <v>0</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="J43" s="52" t="s">
-        <v>244</v>
+        <v>182</v>
+      </c>
+      <c r="J43" s="51" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="48" t="s">
+        <v>251</v>
+      </c>
+      <c r="B44" s="48" t="s">
+        <v>249</v>
+      </c>
+      <c r="C44" s="48" t="s">
+        <v>252</v>
+      </c>
+      <c r="D44" s="48" t="s">
+        <v>252</v>
+      </c>
+      <c r="E44" s="48" t="s">
+        <v>251</v>
+      </c>
+      <c r="F44" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="G44" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="J44" s="52" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>